<commit_message>
update rehab costs for road (now global)
</commit_message>
<xml_diff>
--- a/bundled_data/transport/rehabilitation.xlsx
+++ b/bundled_data/transport/rehabilitation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t xml:space="preserve">Introduction</t>
   </si>
@@ -33,22 +33,28 @@
     <t xml:space="preserve">Sources</t>
   </si>
   <si>
-    <t xml:space="preserve">Roads</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AfDB. Study on Road Infrastructure Costs: Analysis of Unit Costs and Cost Overruns of Road Infrastructure Projects in Africa. AfDB; 2014. </t>
+    <t xml:space="preserve">road</t>
   </si>
   <si>
     <t xml:space="preserve">World Bank. Road Costs Knowledge System (ROCKS) - Doing Business Update. Washington DC: World Bank; 2018. </t>
   </si>
   <si>
+    <t xml:space="preserve">https://collaboration.worldbank.org/content/sites/collaboration-for-development/en/groups/world-bank-road-software-tools.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US Federal Highways Agency, Bridge Replacement Unit Costs 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.fhwa.dot.gov/bridge/nbi/sd2020.cfm#c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.fhwa.dot.gov/bridge/nbi/ascii2022.cfm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Koks EE, Rozenberg J, Zorn C, Tariverdi M, Vousdoukas M, Fraser SA, et al. A global multi-hazard risk analysis of road and railway infrastructure assets. Nature Communications. 2019; 10(1): p. 2677. </t>
   </si>
   <si>
-    <t xml:space="preserve">https://integrum.co.ke/road-construction-costs-per-km-in-kenya-2021/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rail</t>
+    <t xml:space="preserve">rail</t>
   </si>
   <si>
     <t xml:space="preserve">highway</t>
@@ -88,9 +94,6 @@
   </si>
   <si>
     <t xml:space="preserve">cost_USD_per_km</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rail</t>
   </si>
 </sst>
 </file>
@@ -191,7 +194,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -230,6 +233,14 @@
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -309,13 +320,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -327,7 +338,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>2</v>
@@ -340,62 +350,70 @@
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="K5" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="B7" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B8" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5"/>
-      <c r="B13" s="2"/>
-    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E24" s="6"/>
-    </row>
+    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="6"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A5:A8"/>
-  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G6" r:id="rId1" location="c" display="https://www.fhwa.dot.gov/bridge/nbi/sd2020.cfm#c"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -411,181 +429,181 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="24.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="12.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" s="8" t="n">
-        <v>453185</v>
-      </c>
-      <c r="D2" s="2"/>
+        <v>2289717.81609195</v>
+      </c>
+      <c r="D2" s="8"/>
       <c r="E2" s="9"/>
       <c r="F2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="8" t="n">
-        <v>453185</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>23545.1019998726</v>
+      </c>
+      <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" s="8" t="n">
-        <v>453185</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>1312392.31100613</v>
+      </c>
+      <c r="D4" s="8"/>
       <c r="E4" s="9"/>
       <c r="F4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="8" t="n">
-        <v>16031.159786541</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>23545.1019998726</v>
+      </c>
+      <c r="D5" s="8"/>
       <c r="E5" s="5"/>
       <c r="F5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="8" t="n">
-        <v>402906</v>
-      </c>
-      <c r="D6" s="2"/>
+        <v>348280.342022689</v>
+      </c>
+      <c r="D6" s="8"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C7" s="8" t="n">
-        <v>16031.159786541</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>23545.1019998726</v>
+      </c>
+      <c r="D7" s="8"/>
       <c r="E7" s="5"/>
       <c r="F7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="8" t="n">
-        <v>402906</v>
-      </c>
-      <c r="D8" s="2"/>
+        <v>164059.77207298</v>
+      </c>
+      <c r="D8" s="8"/>
       <c r="E8" s="9"/>
       <c r="F8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="8" t="n">
-        <v>13370.3863779865</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>23545.1019998726</v>
+      </c>
+      <c r="D9" s="8"/>
       <c r="E9" s="5"/>
       <c r="F9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C10" s="8" t="n">
-        <v>192972.361390595</v>
-      </c>
-      <c r="D10" s="2"/>
+        <v>164059.77207298</v>
+      </c>
+      <c r="D10" s="8"/>
       <c r="E10" s="5"/>
       <c r="F10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C11" s="8" t="n">
-        <v>13370.3863779865</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>23545.1019998726</v>
+      </c>
+      <c r="D11" s="8"/>
       <c r="E11" s="5"/>
       <c r="F11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="8" t="n">
-        <v>950000</v>
+        <v>15</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>40805816</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="5"/>
@@ -593,17 +611,20 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="8" t="n">
-        <v>16031.159786541</v>
+        <v>16</v>
+      </c>
+      <c r="C13" s="10" t="n">
+        <v>40805816</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="5"/>
       <c r="F13" s="8"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -624,27 +645,27 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>3750000</v>
@@ -654,7 +675,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>37500000</v>

</xml_diff>

<commit_message>
add residential/unclassified road filter file
</commit_message>
<xml_diff>
--- a/bundled_data/transport/rehabilitation.xlsx
+++ b/bundled_data/transport/rehabilitation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t xml:space="preserve">Introduction</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t xml:space="preserve">bridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">residential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unclassified</t>
   </si>
   <si>
     <t xml:space="preserve">asset_type</t>
@@ -326,7 +332,7 @@
       <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -415,8 +421,8 @@
     <hyperlink ref="G6" r:id="rId1" location="c" display="https://www.fhwa.dot.gov/bridge/nbi/sd2020.cfm#c"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -431,11 +437,11 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="24.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="24.87"/>
@@ -623,13 +629,57 @@
       <c r="E13" s="5"/>
       <c r="F13" s="8"/>
     </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="8" t="n">
+        <v>164059.77207298</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="8" t="n">
+        <v>23545.1019998726</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="8" t="n">
+        <v>164059.77207298</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="8" t="n">
+        <v>23545.1019998726</v>
+      </c>
+    </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -644,21 +694,21 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -685,8 +735,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>